<commit_message>
fixed process vocab to have correct options
fixed process_source.xlsx and material_source.xlsx to have correct vocabulary
</commit_message>
<xml_diff>
--- a/utils/excel_files/material_source.xlsx
+++ b/utils/excel_files/material_source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navid\OneDrive\Desktop\MIT\cript-excel-uploader\utils\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873333E7-B1A0-44FF-B18D-5F5DEB74C0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4099F436-8AA9-49FA-B496-CEAE8B00625F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{110CA66B-9233-4308-815F-6679B6D285C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{110CA66B-9233-4308-815F-6679B6D285C8}"/>
   </bookViews>
   <sheets>
     <sheet name="property" sheetId="1" r:id="rId1"/>
@@ -3302,7 +3302,7 @@
   <dimension ref="A1:I157"/>
   <sheetViews>
     <sheetView zoomScale="71" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7716,7 +7716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA6F0B4-BFFA-493D-ABE4-6F7226C201B0}">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -8405,7 +8405,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10354,7 +10354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9ABAB8-9F16-4C85-958F-9BD932FA0E18}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="128" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="128" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
latest update before switching branches
</commit_message>
<xml_diff>
--- a/utils/excel_files/material_source.xlsx
+++ b/utils/excel_files/material_source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navid\OneDrive\Desktop\MIT\cript-excel-uploader\utils\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4099F436-8AA9-49FA-B496-CEAE8B00625F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17D4448-865C-434E-A5C6-E7EF00E7B07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{110CA66B-9233-4308-815F-6679B6D285C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{110CA66B-9233-4308-815F-6679B6D285C8}"/>
   </bookViews>
   <sheets>
     <sheet name="property" sheetId="1" r:id="rId1"/>
@@ -3301,7 +3301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3B6A50-1025-42AE-89F7-24E7EE793A8D}">
   <dimension ref="A1:I157"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -10354,7 +10354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9ABAB8-9F16-4C85-958F-9BD932FA0E18}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="128" workbookViewId="0">
+    <sheetView zoomScale="128" workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>